<commit_message>
All Training and validation data cleaned and merged
</commit_message>
<xml_diff>
--- a/datasets/yearly_death_totals.xlsx
+++ b/datasets/yearly_death_totals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\GitHub\FentanylFighters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\superadmin\cs484\Project\FentanylFighters\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDA4A6E-CCBD-4385-90B6-6C6C950C468D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE3C4AD-E53E-46F2-BF6F-B1F95CDD7905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11250" yWindow="0" windowWidth="11250" windowHeight="15000" xr2:uid="{D125F9EB-F5A0-4639-A64D-32970EB16C29}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D125F9EB-F5A0-4639-A64D-32970EB16C29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBB7C99-DD78-48D3-BFFF-39009E875A2D}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2010</v>
       </c>
@@ -424,8 +424,14 @@
       <c r="K1">
         <v>2020</v>
       </c>
+      <c r="L1">
+        <v>2021</v>
+      </c>
+      <c r="M1">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>19983</v>
       </c>
@@ -458,6 +464,12 @@
       </c>
       <c r="K2">
         <v>69432</v>
+      </c>
+      <c r="L2">
+        <v>81415</v>
+      </c>
+      <c r="M2">
+        <v>76633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>